<commit_message>
Added function to reconvert to frames and conform to Hulu and YouTube needs.
</commit_message>
<xml_diff>
--- a/timecodesFrames.xlsx
+++ b/timecodesFrames.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="2093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="2097">
   <si>
     <t>Timecode</t>
   </si>
@@ -6299,6 +6299,18 @@
   </si>
   <si>
     <t>01:08:41;12</t>
+  </si>
+  <si>
+    <t>01:15:22:08</t>
+  </si>
+  <si>
+    <t>01:21:57:18</t>
+  </si>
+  <si>
+    <t>01:28:58:15</t>
+  </si>
+  <si>
+    <t>01:36:08:06</t>
   </si>
 </sst>
 </file>
@@ -6376,9 +6388,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="58">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6444,7 +6462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="58">
+  <cellStyles count="64">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -6474,6 +6492,9 @@
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -6502,6 +6523,9 @@
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -6853,10 +6877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7969,6 +7993,420 @@
       <c r="U30">
         <f>VALUE(LEFT(A30,2))*60*60*25+VALUE(MID(A30,4,2))*60*25+VALUE(MID(A30,7,2))*25+RIGHT(A30,2)</f>
         <v>103037</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B32" t="str">
+        <f>LEFT(A32,2)</f>
+        <v>01</v>
+      </c>
+      <c r="C32" t="str">
+        <f>MID(A32,4,2)</f>
+        <v>15</v>
+      </c>
+      <c r="D32" t="str">
+        <f>MID(A32,7,2)</f>
+        <v>22</v>
+      </c>
+      <c r="E32" t="str">
+        <f>RIGHT(A32,2)</f>
+        <v>08</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1">
+        <f>VALUE(B32)*60*60*25</f>
+        <v>90000</v>
+      </c>
+      <c r="H32" s="1">
+        <f>VALUE(C32)*60*25</f>
+        <v>22500</v>
+      </c>
+      <c r="I32" s="1">
+        <f>VALUE(D32)*25</f>
+        <v>550</v>
+      </c>
+      <c r="J32" s="1">
+        <f>G32+H32+I32+E32</f>
+        <v>113058</v>
+      </c>
+      <c r="L32">
+        <v>23058</v>
+      </c>
+      <c r="M32">
+        <f>MOD(INT(INT(INT(ABS(L32)/25)/60)/60),60)</f>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f>MOD(INT(INT(ABS(L32)/25)/60),60)</f>
+        <v>15</v>
+      </c>
+      <c r="O32" s="2">
+        <f>MOD(INT(ABS(L32)/25),60)</f>
+        <v>22</v>
+      </c>
+      <c r="P32" s="2">
+        <f>MOD(ABS(L32),25)</f>
+        <v>8</v>
+      </c>
+      <c r="R32" t="str">
+        <f>TEXT(M32,"00")&amp;":"&amp;TEXT(N32,"00")&amp;":"&amp;TEXT(O32,"00")&amp;";"&amp;TEXT(P32,"00")</f>
+        <v>00:15:22;08</v>
+      </c>
+      <c r="T32" t="str">
+        <f>TEXT(MOD(INT(INT(INT(ABS(L32)/25)/60)/60),60),"00")&amp;":"&amp;TEXT(MOD(INT(INT(ABS(L32)/25)/60),60),"00")&amp;":"&amp;TEXT(MOD(INT(ABS(L32)/25),60),"00")&amp;";"&amp;TEXT(MOD(ABS(L32),25),"00")</f>
+        <v>00:15:22;08</v>
+      </c>
+      <c r="U32">
+        <f>VALUE(LEFT(A32,2))*60*60*25+VALUE(MID(A32,4,2))*60*25+VALUE(MID(A32,7,2))*25+RIGHT(A32,2)</f>
+        <v>113058</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" ref="B37:B41" si="7">LEFT(A37,2)</f>
+        <v>01</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" ref="C37:C41" si="8">MID(A37,4,2)</f>
+        <v>08</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D37:D41" si="9">MID(A37,7,2)</f>
+        <v>40</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" ref="E37:E41" si="10">RIGHT(A37,2)</f>
+        <v>12</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="1">
+        <f t="shared" ref="G37:G41" si="11">VALUE(B37)*60*60*25</f>
+        <v>90000</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" ref="H37:H41" si="12">VALUE(C37)*60*25</f>
+        <v>12000</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" ref="I37:I41" si="13">VALUE(D37)*25</f>
+        <v>1000</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" ref="J37:J41" si="14">G37+H37+I37+E37</f>
+        <v>103012</v>
+      </c>
+      <c r="L37">
+        <v>13012</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ref="M37:M41" si="15">MOD(INT(INT(INT(ABS(L37)/25)/60)/60),60)</f>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:N41" si="16">MOD(INT(INT(ABS(L37)/25)/60),60)</f>
+        <v>8</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" ref="O37:O41" si="17">MOD(INT(ABS(L37)/25),60)</f>
+        <v>40</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" ref="P37:P41" si="18">MOD(ABS(L37),25)</f>
+        <v>12</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" ref="R37:R41" si="19">TEXT(M37,"00")&amp;":"&amp;TEXT(N37,"00")&amp;":"&amp;TEXT(O37,"00")&amp;";"&amp;TEXT(P37,"00")</f>
+        <v>00:08:40;12</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" ref="T37:T41" si="20">TEXT(MOD(INT(INT(INT(ABS(L37)/25)/60)/60),60),"00")&amp;":"&amp;TEXT(MOD(INT(INT(ABS(L37)/25)/60),60),"00")&amp;":"&amp;TEXT(MOD(INT(ABS(L37)/25),60),"00")&amp;";"&amp;TEXT(MOD(ABS(L37),25),"00")</f>
+        <v>00:08:40;12</v>
+      </c>
+      <c r="U37">
+        <f t="shared" ref="U37:U41" si="21">VALUE(LEFT(A37,2))*60*60*25+VALUE(MID(A37,4,2))*60*25+VALUE(MID(A37,7,2))*25+RIGHT(A37,2)</f>
+        <v>103012</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="7"/>
+        <v>01</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="10"/>
+        <v>08</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="1">
+        <f t="shared" si="11"/>
+        <v>90000</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="12"/>
+        <v>22500</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="13"/>
+        <v>550</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="14"/>
+        <v>113058</v>
+      </c>
+      <c r="L38">
+        <v>23058</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="17"/>
+        <v>22</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="19"/>
+        <v>00:15:22;08</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="20"/>
+        <v>00:15:22;08</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="21"/>
+        <v>113058</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="7"/>
+        <v>01</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="9"/>
+        <v>57</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="1">
+        <f t="shared" si="11"/>
+        <v>90000</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="12"/>
+        <v>31500</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="13"/>
+        <v>1425</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="14"/>
+        <v>122943</v>
+      </c>
+      <c r="L39">
+        <v>32943</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="16"/>
+        <v>21</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="17"/>
+        <v>57</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="19"/>
+        <v>00:21:57;18</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="20"/>
+        <v>00:21:57;18</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="21"/>
+        <v>122943</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="7"/>
+        <v>01</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="9"/>
+        <v>58</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="1">
+        <f t="shared" si="11"/>
+        <v>90000</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="12"/>
+        <v>42000</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="13"/>
+        <v>1450</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="14"/>
+        <v>133465</v>
+      </c>
+      <c r="L40">
+        <v>43465</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="17"/>
+        <v>58</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="19"/>
+        <v>00:28:58;15</v>
+      </c>
+      <c r="T40" t="str">
+        <f t="shared" si="20"/>
+        <v>00:28:58;15</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="21"/>
+        <v>133465</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="7"/>
+        <v>01</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="9"/>
+        <v>08</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="10"/>
+        <v>06</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="1">
+        <f t="shared" si="11"/>
+        <v>90000</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="12"/>
+        <v>54000</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="13"/>
+        <v>200</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="14"/>
+        <v>144206</v>
+      </c>
+      <c r="L41">
+        <v>54206</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="16"/>
+        <v>36</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="19"/>
+        <v>00:36:08;06</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="20"/>
+        <v>00:36:08;06</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="21"/>
+        <v>144206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>